<commit_message>
add special method text for tuolumne floodplain
</commit_message>
<xml_diff>
--- a/data-raw/CVPIA_FloodplainAreas_docs.xlsx
+++ b/data-raw/CVPIA_FloodplainAreas_docs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DocTemplate" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,11 +13,6 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">R_Ready!$F$1:$F$1017</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">R_Ready!$F$1:$F$1017</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">R_Ready!$F$1:$F$1017</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">R_Ready!$F$1:$F$1017</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">R_Ready!$F$1:$F$1017</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">R_Ready!$F$1:$F$1017</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="113">
   <si>
     <t xml:space="preserve">method</t>
   </si>
@@ -317,6 +312,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tuolumne River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">full_model_t</t>
   </si>
   <si>
     <t xml:space="preserve">TUFLOW hydraulic model with 1D channel and 2D overbank components</t>
@@ -622,18 +620,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="50.5587044534413"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="52.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="50.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -778,7 +778,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -791,24 +791,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB65536"/>
+  <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.3481781376518"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="37.4898785425101"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="15" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="37.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2901,10 +2906,10 @@
         <v>95</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>69</v>
@@ -2992,16 +2997,16 @@
     </row>
     <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>23.072031</v>
@@ -3086,16 +3091,16 @@
     </row>
     <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>59.18568</v>
@@ -3115,16 +3120,16 @@
     </row>
     <row r="28" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>122.450036</v>
@@ -3144,16 +3149,16 @@
     </row>
     <row r="29" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>57.96251</v>
@@ -3173,16 +3178,16 @@
     </row>
     <row r="30" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E30" s="3" t="n">
         <v>13.702192</v>
@@ -3202,16 +3207,16 @@
     </row>
     <row r="31" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>45.654083</v>
@@ -3231,16 +3236,16 @@
     </row>
     <row r="32" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="D32" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>69.617216</v>
@@ -3260,16 +3265,16 @@
     </row>
     <row r="33" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6" t="n">
@@ -3284,16 +3289,16 @@
     </row>
     <row r="34" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6" t="n">
@@ -3336,7 +3341,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>